<commit_message>
Working on reading multiple items
</commit_message>
<xml_diff>
--- a/SubClassesWW2/PreWork.xlsx
+++ b/SubClassesWW2/PreWork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PythonExercises\SubClassesWW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288D7C2D-4336-4E5E-9EE4-E169FDB72314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1741EEB2-4F3E-47A8-8633-78510E1C77A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>FROM:</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Black Swan-class sloop</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/British_S-class_submarine_(1931)</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1134,7 +1137,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1398,13 +1401,12 @@
       <c r="C22" t="str">
         <v>British S-class submarine</v>
       </c>
-      <c r="D22" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.wikipedia.org/wiki/British S-class submarine</v>
+      <c r="D22" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>'https://www.wikipedia.org/wiki/British S-class submarine',</v>
+        <v>'https://en.wikipedia.org/wiki/British_S-class_submarine_(1931)',</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1499,8 +1501,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D22" r:id="rId1" xr:uid="{091396DA-F498-458F-92C5-0B1B36DADED2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1542,7 +1547,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Dec-2023</v>
+        <v>14-Dec-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1838,7 +1843,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Dec-2023</v>
+        <v>14-Dec-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>